<commit_message>
gw: update oncho forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Guinea Bissau/gw_oncho_202302_prestop_1_site.xlsx
+++ b/ONCHO/Impact Assessments/Guinea Bissau/gw_oncho_202302_prestop_1_site.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\ONCHO\Impact Assessments\Guinea Bissau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B1EE0E-F88D-499A-97F7-E3BA6385334D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EB363A-2ACA-4F6F-8955-4F559C3D3AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -960,7 +960,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1666,9 +1676,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G289"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B293" sqref="B293"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2239,14 +2249,14 @@
       <c r="A35" t="s">
         <v>53</v>
       </c>
-      <c r="B35" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" t="s">
-        <v>126</v>
+      <c r="B35" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D35" t="s">
-        <v>126</v>
+        <v>211</v>
       </c>
       <c r="F35" t="s">
         <v>70</v>
@@ -2257,16 +2267,16 @@
         <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="D36" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="F36" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2274,13 +2284,13 @@
         <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D37" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F37" t="s">
         <v>88</v>
@@ -2291,13 +2301,13 @@
         <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C38" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F38" t="s">
         <v>88</v>
@@ -2308,13 +2318,13 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="C39" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="F39" t="s">
         <v>88</v>
@@ -2324,14 +2334,14 @@
       <c r="A40" t="s">
         <v>53</v>
       </c>
-      <c r="B40" t="s">
-        <v>202</v>
-      </c>
-      <c r="C40" t="s">
-        <v>202</v>
+      <c r="B40" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D40" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="F40" t="s">
         <v>88</v>
@@ -2342,16 +2352,16 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="D41" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="F41" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2359,16 +2369,16 @@
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="C42" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="D42" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="F42" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2376,16 +2386,16 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="D43" t="s">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="F43" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2393,13 +2403,13 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="D44" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="F44" t="s">
         <v>86</v>
@@ -2410,13 +2420,13 @@
         <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="C45" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D45" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="F45" t="s">
         <v>86</v>
@@ -2427,13 +2437,13 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="C46" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D46" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="F46" t="s">
         <v>86</v>
@@ -2444,13 +2454,13 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="D47" t="s">
-        <v>183</v>
+        <v>89</v>
       </c>
       <c r="F47" t="s">
         <v>86</v>
@@ -2460,14 +2470,14 @@
       <c r="A48" t="s">
         <v>53</v>
       </c>
-      <c r="B48" t="s">
-        <v>200</v>
-      </c>
-      <c r="C48" t="s">
-        <v>200</v>
+      <c r="B48" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="F48" t="s">
         <v>86</v>
@@ -2478,13 +2488,13 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D49" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="F49" t="s">
         <v>86</v>
@@ -2495,16 +2505,16 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="F50" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2512,16 +2522,16 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="D51" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="F51" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2529,16 +2539,16 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
+        <v>200</v>
       </c>
       <c r="F52" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2546,16 +2556,16 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="C53" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="D53" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="F53" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2563,13 +2573,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C54" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D54" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F54" t="s">
         <v>79</v>
@@ -2580,13 +2590,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D55" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F55" t="s">
         <v>79</v>
@@ -2597,13 +2607,13 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="F56" t="s">
         <v>79</v>
@@ -2614,13 +2624,13 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="C57" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="F57" t="s">
         <v>79</v>
@@ -2631,13 +2641,13 @@
         <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="C58" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="D58" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="F58" t="s">
         <v>79</v>
@@ -2648,13 +2658,13 @@
         <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="C59" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="F59" t="s">
         <v>79</v>
@@ -2665,13 +2675,13 @@
         <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="C60" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="D60" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="F60" t="s">
         <v>79</v>
@@ -2682,33 +2692,33 @@
         <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="C61" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="D61" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="F61" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>53</v>
       </c>
-      <c r="B62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" t="s">
-        <v>128</v>
+      <c r="B62" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D62" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="F62" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2716,16 +2726,16 @@
         <v>53</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="C63" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="D63" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="F63" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2733,16 +2743,16 @@
         <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="C64" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="D64" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="F64" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2750,16 +2760,16 @@
         <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="D65" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="F65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2767,33 +2777,33 @@
         <v>53</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="F66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>53</v>
       </c>
-      <c r="B67" t="s">
-        <v>167</v>
-      </c>
-      <c r="C67" t="s">
-        <v>167</v>
+      <c r="B67" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D67" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="F67" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2801,13 +2811,13 @@
         <v>53</v>
       </c>
       <c r="B68" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="C68" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="D68" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="F68" t="s">
         <v>78</v>
@@ -2818,13 +2828,13 @@
         <v>53</v>
       </c>
       <c r="B69" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="C69" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="D69" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="F69" t="s">
         <v>78</v>
@@ -2835,13 +2845,13 @@
         <v>53</v>
       </c>
       <c r="B70" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C70" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D70" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F70" t="s">
         <v>78</v>
@@ -2852,13 +2862,13 @@
         <v>53</v>
       </c>
       <c r="B71" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="D71" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="F71" t="s">
         <v>78</v>
@@ -2869,13 +2879,13 @@
         <v>53</v>
       </c>
       <c r="B72" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="C72" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="D72" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="F72" t="s">
         <v>78</v>
@@ -2886,16 +2896,16 @@
         <v>53</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C73" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D73" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F73" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2903,16 +2913,16 @@
         <v>53</v>
       </c>
       <c r="B74" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="C74" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="D74" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="F74" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2920,33 +2930,33 @@
         <v>53</v>
       </c>
       <c r="B75" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C75" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="D75" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="F75" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>53</v>
       </c>
-      <c r="B76" t="s">
-        <v>110</v>
-      </c>
-      <c r="C76" t="s">
-        <v>110</v>
+      <c r="B76" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D76" t="s">
-        <v>110</v>
+        <v>211</v>
       </c>
       <c r="F76" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2954,16 +2964,16 @@
         <v>53</v>
       </c>
       <c r="B77" t="s">
-        <v>112</v>
+        <v>204</v>
       </c>
       <c r="C77" t="s">
-        <v>112</v>
+        <v>204</v>
       </c>
       <c r="D77" t="s">
-        <v>112</v>
+        <v>204</v>
       </c>
       <c r="F77" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2971,16 +2981,16 @@
         <v>53</v>
       </c>
       <c r="B78" t="s">
-        <v>113</v>
+        <v>205</v>
       </c>
       <c r="C78" t="s">
-        <v>113</v>
+        <v>205</v>
       </c>
       <c r="D78" t="s">
-        <v>113</v>
+        <v>205</v>
       </c>
       <c r="F78" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2988,16 +2998,16 @@
         <v>53</v>
       </c>
       <c r="B79" t="s">
-        <v>119</v>
+        <v>206</v>
       </c>
       <c r="C79" t="s">
-        <v>119</v>
+        <v>206</v>
       </c>
       <c r="D79" t="s">
-        <v>119</v>
+        <v>206</v>
       </c>
       <c r="F79" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3005,33 +3015,33 @@
         <v>53</v>
       </c>
       <c r="B80" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="C80" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="D80" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="F80" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>53</v>
       </c>
-      <c r="B81" t="s">
-        <v>121</v>
-      </c>
-      <c r="C81" t="s">
-        <v>121</v>
+      <c r="B81" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D81" t="s">
-        <v>121</v>
+        <v>211</v>
       </c>
       <c r="F81" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3039,16 +3049,16 @@
         <v>53</v>
       </c>
       <c r="B82" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="C82" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="D82" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="F82" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3056,16 +3066,16 @@
         <v>53</v>
       </c>
       <c r="B83" t="s">
-        <v>140</v>
+        <v>193</v>
       </c>
       <c r="C83" t="s">
-        <v>140</v>
+        <v>193</v>
       </c>
       <c r="D83" t="s">
-        <v>140</v>
+        <v>193</v>
       </c>
       <c r="F83" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3073,16 +3083,16 @@
         <v>53</v>
       </c>
       <c r="B84" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="C84" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="D84" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="F84" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3090,16 +3100,16 @@
         <v>53</v>
       </c>
       <c r="B85" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="C85" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="D85" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="F85" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3107,16 +3117,16 @@
         <v>53</v>
       </c>
       <c r="B86" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C86" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D86" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F86" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3124,33 +3134,33 @@
         <v>53</v>
       </c>
       <c r="B87" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="C87" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="D87" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="F87" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>53</v>
       </c>
-      <c r="B88" t="s">
-        <v>159</v>
-      </c>
-      <c r="C88" t="s">
-        <v>159</v>
+      <c r="B88" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C88" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D88" t="s">
-        <v>159</v>
+        <v>211</v>
       </c>
       <c r="F88" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3158,16 +3168,16 @@
         <v>53</v>
       </c>
       <c r="B89" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
       <c r="C89" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
       <c r="D89" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
       <c r="F89" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3175,16 +3185,16 @@
         <v>53</v>
       </c>
       <c r="B90" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="C90" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="D90" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="F90" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3192,13 +3202,13 @@
         <v>53</v>
       </c>
       <c r="B91" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="C91" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="D91" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="F91" t="s">
         <v>81</v>
@@ -3209,13 +3219,13 @@
         <v>53</v>
       </c>
       <c r="B92" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
       <c r="C92" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
       <c r="D92" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
       <c r="F92" t="s">
         <v>81</v>
@@ -3226,13 +3236,13 @@
         <v>53</v>
       </c>
       <c r="B93" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="D93" t="s">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="F93" t="s">
         <v>81</v>
@@ -3243,13 +3253,13 @@
         <v>53</v>
       </c>
       <c r="B94" t="s">
-        <v>199</v>
+        <v>145</v>
       </c>
       <c r="C94" t="s">
-        <v>199</v>
+        <v>145</v>
       </c>
       <c r="D94" t="s">
-        <v>199</v>
+        <v>145</v>
       </c>
       <c r="F94" t="s">
         <v>81</v>
@@ -3260,13 +3270,13 @@
         <v>53</v>
       </c>
       <c r="B95" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="C95" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="D95" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="F95" t="s">
         <v>81</v>
@@ -3277,16 +3287,16 @@
         <v>53</v>
       </c>
       <c r="B96" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="C96" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="D96" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="F96" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3294,16 +3304,16 @@
         <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C97" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D97" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="F97" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3311,16 +3321,16 @@
         <v>53</v>
       </c>
       <c r="B98" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="C98" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="D98" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="F98" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3328,16 +3338,16 @@
         <v>53</v>
       </c>
       <c r="B99" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="C99" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="D99" t="s">
-        <v>105</v>
+        <v>169</v>
       </c>
       <c r="F99" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3345,33 +3355,33 @@
         <v>53</v>
       </c>
       <c r="B100" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="C100" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="D100" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="F100" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>53</v>
       </c>
-      <c r="B101" t="s">
-        <v>97</v>
-      </c>
-      <c r="C101" t="s">
-        <v>97</v>
+      <c r="B101" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C101" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D101" t="s">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="F101" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3379,16 +3389,16 @@
         <v>53</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="C102" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="D102" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="F102" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -3396,16 +3406,16 @@
         <v>53</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
+        <v>239</v>
       </c>
       <c r="C103" t="s">
-        <v>101</v>
+        <v>239</v>
       </c>
       <c r="D103" t="s">
-        <v>101</v>
+        <v>239</v>
       </c>
       <c r="F103" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3413,16 +3423,16 @@
         <v>53</v>
       </c>
       <c r="B104" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="C104" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="D104" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="F104" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3430,16 +3440,16 @@
         <v>53</v>
       </c>
       <c r="B105" t="s">
-        <v>103</v>
+        <v>199</v>
       </c>
       <c r="C105" t="s">
-        <v>103</v>
+        <v>199</v>
       </c>
       <c r="D105" t="s">
-        <v>103</v>
+        <v>199</v>
       </c>
       <c r="F105" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3447,16 +3457,16 @@
         <v>53</v>
       </c>
       <c r="B106" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="C106" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="D106" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="F106" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3464,16 +3474,16 @@
         <v>53</v>
       </c>
       <c r="B107" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="C107" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="D107" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="F107" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3481,33 +3491,33 @@
         <v>53</v>
       </c>
       <c r="B108" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="C108" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="D108" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="F108" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>53</v>
       </c>
-      <c r="B109" t="s">
-        <v>190</v>
-      </c>
-      <c r="C109" t="s">
-        <v>190</v>
+      <c r="B109" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D109" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="F109" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3515,16 +3525,16 @@
         <v>53</v>
       </c>
       <c r="B110" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C110" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="D110" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="F110" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3532,16 +3542,16 @@
         <v>53</v>
       </c>
       <c r="B111" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="C111" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="D111" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="F111" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3549,16 +3559,16 @@
         <v>53</v>
       </c>
       <c r="B112" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C112" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D112" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F112" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3566,16 +3576,16 @@
         <v>53</v>
       </c>
       <c r="B113" t="s">
-        <v>174</v>
+        <v>102</v>
       </c>
       <c r="C113" t="s">
-        <v>174</v>
+        <v>102</v>
       </c>
       <c r="D113" t="s">
-        <v>174</v>
+        <v>102</v>
       </c>
       <c r="F113" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3583,16 +3593,16 @@
         <v>53</v>
       </c>
       <c r="B114" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C114" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D114" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F114" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3600,33 +3610,33 @@
         <v>53</v>
       </c>
       <c r="B115" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C115" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D115" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F115" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>53</v>
       </c>
-      <c r="B116" t="s">
-        <v>132</v>
-      </c>
-      <c r="C116" t="s">
-        <v>132</v>
+      <c r="B116" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C116" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D116" t="s">
-        <v>132</v>
+        <v>211</v>
       </c>
       <c r="F116" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3634,16 +3644,16 @@
         <v>53</v>
       </c>
       <c r="B117" t="s">
-        <v>133</v>
+        <v>186</v>
       </c>
       <c r="C117" t="s">
-        <v>133</v>
+        <v>186</v>
       </c>
       <c r="D117" t="s">
-        <v>133</v>
+        <v>186</v>
       </c>
       <c r="F117" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3651,16 +3661,16 @@
         <v>53</v>
       </c>
       <c r="B118" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="C118" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="D118" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="F118" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3668,16 +3678,16 @@
         <v>53</v>
       </c>
       <c r="B119" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="C119" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="D119" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="F119" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3685,16 +3695,16 @@
         <v>53</v>
       </c>
       <c r="B120" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="C120" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="D120" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="F120" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3702,33 +3712,33 @@
         <v>53</v>
       </c>
       <c r="B121" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="C121" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="D121" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="F121" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>53</v>
       </c>
-      <c r="B122" t="s">
-        <v>170</v>
-      </c>
-      <c r="C122" t="s">
-        <v>170</v>
+      <c r="B122" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C122" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D122" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="F122" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3736,33 +3746,33 @@
         <v>53</v>
       </c>
       <c r="B123" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="C123" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="D123" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="F123" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>53</v>
       </c>
-      <c r="B124" t="s">
-        <v>173</v>
-      </c>
-      <c r="C124" t="s">
-        <v>173</v>
+      <c r="B124" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C124" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D124" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="F124" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3770,16 +3780,16 @@
         <v>53</v>
       </c>
       <c r="B125" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="C125" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="D125" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="F125" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3787,33 +3797,33 @@
         <v>53</v>
       </c>
       <c r="B126" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C126" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D126" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F126" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>53</v>
       </c>
-      <c r="B127" t="s">
-        <v>196</v>
-      </c>
-      <c r="C127" t="s">
-        <v>196</v>
+      <c r="B127" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C127" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D127" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="F127" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3821,16 +3831,16 @@
         <v>53</v>
       </c>
       <c r="B128" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C128" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D128" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="F128" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3838,33 +3848,33 @@
         <v>53</v>
       </c>
       <c r="B129" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="C129" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="D129" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="F129" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>53</v>
       </c>
-      <c r="B130" t="s">
-        <v>122</v>
-      </c>
-      <c r="C130" t="s">
-        <v>122</v>
+      <c r="B130" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D130" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
       <c r="F130" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3872,16 +3882,16 @@
         <v>53</v>
       </c>
       <c r="B131" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C131" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D131" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="F131" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3889,16 +3899,16 @@
         <v>53</v>
       </c>
       <c r="B132" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C132" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D132" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F132" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3906,16 +3916,16 @@
         <v>53</v>
       </c>
       <c r="B133" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C133" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D133" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F133" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3923,16 +3933,16 @@
         <v>53</v>
       </c>
       <c r="B134" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C134" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D134" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="F134" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3940,16 +3950,16 @@
         <v>53</v>
       </c>
       <c r="B135" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
       <c r="C135" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
       <c r="D135" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
       <c r="F135" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3957,16 +3967,16 @@
         <v>53</v>
       </c>
       <c r="B136" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C136" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D136" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F136" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3974,16 +3984,16 @@
         <v>53</v>
       </c>
       <c r="B137" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="C137" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="D137" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="F137" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3991,16 +4001,16 @@
         <v>53</v>
       </c>
       <c r="B138" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="C138" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="D138" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="F138" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -4008,16 +4018,16 @@
         <v>53</v>
       </c>
       <c r="B139" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="C139" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="D139" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="F139" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -4025,33 +4035,33 @@
         <v>53</v>
       </c>
       <c r="B140" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="C140" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="D140" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="F140" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>53</v>
       </c>
-      <c r="B141" t="s">
-        <v>148</v>
-      </c>
-      <c r="C141" t="s">
-        <v>148</v>
+      <c r="B141" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C141" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D141" t="s">
-        <v>148</v>
+        <v>211</v>
       </c>
       <c r="F141" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -4059,16 +4069,16 @@
         <v>53</v>
       </c>
       <c r="B142" t="s">
-        <v>92</v>
+        <v>184</v>
       </c>
       <c r="C142" t="s">
-        <v>92</v>
+        <v>184</v>
       </c>
       <c r="D142" t="s">
-        <v>92</v>
+        <v>184</v>
       </c>
       <c r="F142" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -4076,16 +4086,16 @@
         <v>53</v>
       </c>
       <c r="B143" t="s">
-        <v>107</v>
+        <v>196</v>
       </c>
       <c r="C143" t="s">
-        <v>107</v>
+        <v>196</v>
       </c>
       <c r="D143" t="s">
-        <v>107</v>
+        <v>196</v>
       </c>
       <c r="F143" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -4093,16 +4103,16 @@
         <v>53</v>
       </c>
       <c r="B144" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C144" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D144" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F144" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4110,33 +4120,33 @@
         <v>53</v>
       </c>
       <c r="B145" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C145" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D145" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F145" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>53</v>
       </c>
-      <c r="B146" t="s">
-        <v>116</v>
-      </c>
-      <c r="C146" t="s">
-        <v>116</v>
+      <c r="B146" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C146" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D146" t="s">
-        <v>116</v>
+        <v>211</v>
       </c>
       <c r="F146" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -4144,16 +4154,16 @@
         <v>53</v>
       </c>
       <c r="B147" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C147" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D147" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F147" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -4161,101 +4171,101 @@
         <v>53</v>
       </c>
       <c r="B148" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C148" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D148" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F148" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>53</v>
       </c>
-      <c r="B149" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C149" s="16" t="s">
-        <v>208</v>
+      <c r="B149" t="s">
+        <v>127</v>
+      </c>
+      <c r="C149" t="s">
+        <v>127</v>
       </c>
       <c r="D149" t="s">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="F149" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>53</v>
       </c>
-      <c r="B150" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C150" s="16" t="s">
-        <v>208</v>
+      <c r="B150" t="s">
+        <v>152</v>
+      </c>
+      <c r="C150" t="s">
+        <v>152</v>
       </c>
       <c r="D150" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
       <c r="F150" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>53</v>
       </c>
-      <c r="B151" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C151" s="16" t="s">
-        <v>208</v>
+      <c r="B151" t="s">
+        <v>164</v>
+      </c>
+      <c r="C151" t="s">
+        <v>164</v>
       </c>
       <c r="D151" t="s">
-        <v>211</v>
+        <v>164</v>
       </c>
       <c r="F151" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>53</v>
       </c>
-      <c r="B152" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C152" s="16" t="s">
-        <v>208</v>
+      <c r="B152" t="s">
+        <v>240</v>
+      </c>
+      <c r="C152" t="s">
+        <v>240</v>
       </c>
       <c r="D152" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="F152" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>53</v>
       </c>
-      <c r="B153" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C153" s="16" t="s">
-        <v>208</v>
+      <c r="B153" t="s">
+        <v>177</v>
+      </c>
+      <c r="C153" t="s">
+        <v>177</v>
       </c>
       <c r="D153" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="F153" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -4272,58 +4282,58 @@
         <v>211</v>
       </c>
       <c r="F154" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>53</v>
       </c>
-      <c r="B155" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C155" s="16" t="s">
-        <v>208</v>
+      <c r="B155" t="s">
+        <v>192</v>
+      </c>
+      <c r="C155" t="s">
+        <v>192</v>
       </c>
       <c r="D155" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="F155" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>53</v>
       </c>
-      <c r="B156" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C156" s="16" t="s">
-        <v>208</v>
+      <c r="B156" t="s">
+        <v>197</v>
+      </c>
+      <c r="C156" t="s">
+        <v>197</v>
       </c>
       <c r="D156" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="F156" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>53</v>
       </c>
-      <c r="B157" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C157" s="16" t="s">
-        <v>208</v>
+      <c r="B157" t="s">
+        <v>109</v>
+      </c>
+      <c r="C157" t="s">
+        <v>109</v>
       </c>
       <c r="D157" t="s">
-        <v>211</v>
+        <v>109</v>
       </c>
       <c r="F157" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -4340,41 +4350,41 @@
         <v>211</v>
       </c>
       <c r="F158" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>53</v>
       </c>
-      <c r="B159" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C159" s="16" t="s">
-        <v>208</v>
+      <c r="B159" t="s">
+        <v>143</v>
+      </c>
+      <c r="C159" t="s">
+        <v>143</v>
       </c>
       <c r="D159" t="s">
-        <v>211</v>
+        <v>143</v>
       </c>
       <c r="F159" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>53</v>
       </c>
-      <c r="B160" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C160" s="16" t="s">
-        <v>208</v>
+      <c r="B160" t="s">
+        <v>148</v>
+      </c>
+      <c r="C160" t="s">
+        <v>148</v>
       </c>
       <c r="D160" t="s">
-        <v>211</v>
+        <v>148</v>
       </c>
       <c r="F160" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -4391,109 +4401,109 @@
         <v>211</v>
       </c>
       <c r="F161" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" t="s">
         <v>53</v>
       </c>
-      <c r="B162" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C162" s="16" t="s">
-        <v>208</v>
+      <c r="B162" t="s">
+        <v>92</v>
+      </c>
+      <c r="C162" t="s">
+        <v>92</v>
       </c>
       <c r="D162" t="s">
-        <v>211</v>
+        <v>92</v>
       </c>
       <c r="F162" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="163" spans="1:7">
       <c r="A163" t="s">
         <v>53</v>
       </c>
-      <c r="B163" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C163" s="16" t="s">
-        <v>208</v>
+      <c r="B163" t="s">
+        <v>107</v>
+      </c>
+      <c r="C163" t="s">
+        <v>107</v>
       </c>
       <c r="D163" t="s">
-        <v>211</v>
+        <v>107</v>
       </c>
       <c r="F163" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="164" spans="1:7">
       <c r="A164" t="s">
         <v>53</v>
       </c>
-      <c r="B164" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C164" s="16" t="s">
-        <v>208</v>
+      <c r="B164" t="s">
+        <v>108</v>
+      </c>
+      <c r="C164" t="s">
+        <v>108</v>
       </c>
       <c r="D164" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="F164" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="165" spans="1:7">
       <c r="A165" t="s">
         <v>53</v>
       </c>
-      <c r="B165" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C165" s="16" t="s">
-        <v>208</v>
+      <c r="B165" t="s">
+        <v>111</v>
+      </c>
+      <c r="C165" t="s">
+        <v>111</v>
       </c>
       <c r="D165" t="s">
-        <v>211</v>
+        <v>111</v>
       </c>
       <c r="F165" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="166" spans="1:7">
       <c r="A166" t="s">
         <v>53</v>
       </c>
-      <c r="B166" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C166" s="16" t="s">
-        <v>208</v>
+      <c r="B166" t="s">
+        <v>116</v>
+      </c>
+      <c r="C166" t="s">
+        <v>116</v>
       </c>
       <c r="D166" t="s">
-        <v>211</v>
+        <v>116</v>
       </c>
       <c r="F166" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="167" spans="1:7">
       <c r="A167" t="s">
         <v>53</v>
       </c>
-      <c r="B167" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C167" s="16" t="s">
-        <v>208</v>
+      <c r="B167" t="s">
+        <v>120</v>
+      </c>
+      <c r="C167" t="s">
+        <v>120</v>
       </c>
       <c r="D167" t="s">
-        <v>211</v>
+        <v>120</v>
       </c>
       <c r="F167" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -4510,24 +4520,24 @@
         <v>211</v>
       </c>
       <c r="F168" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="169" spans="1:7">
       <c r="A169" t="s">
         <v>53</v>
       </c>
-      <c r="B169" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C169" s="16" t="s">
-        <v>208</v>
+      <c r="B169" t="s">
+        <v>125</v>
+      </c>
+      <c r="C169" t="s">
+        <v>125</v>
       </c>
       <c r="D169" t="s">
-        <v>211</v>
+        <v>125</v>
       </c>
       <c r="F169" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -6554,9 +6564,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:F28">
-    <sortCondition ref="A21:A28"/>
-    <sortCondition ref="F21:F28"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:G169">
+    <sortCondition ref="F30:F169"/>
+    <sortCondition ref="B30:B169"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6566,8 +6576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6615,8 +6625,8 @@
   <dimension ref="B1:M120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D120"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -8458,7 +8468,7 @@
         <v>77</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>97</v>
@@ -8538,7 +8548,7 @@
         <v>77</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>103</v>

</xml_diff>